<commit_message>
Single whitlisted function for both templated and raw file
</commit_message>
<xml_diff>
--- a/frappe/core/doctype/data_import/test_data/test_xlsx_file.xlsx
+++ b/frappe/core/doctype/data_import/test_data/test_xlsx_file.xlsx
@@ -244,21 +244,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -382,40 +382,23 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>9638527410</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>8521479632</v>
+        <v>9638527410</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>10</v>
@@ -423,19 +406,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>8547963214</v>
+        <v>8521479632</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>10</v>
@@ -443,41 +426,64 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>8547963214</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B12" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="0" t="n">
+      <c r="C12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>8745632109</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="F12" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B13" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>9856743012</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>